<commit_message>
Finishing up calculating LP averages
</commit_message>
<xml_diff>
--- a/Plastics ingestion records fish master_UDPATED_AGM-MSS2.xlsx
+++ b/Plastics ingestion records fish master_UDPATED_AGM-MSS2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/test/Box Sync/Microplastics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/test/Box Sync/Microplastics/Fish-plastics-meta-analysis-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA1A7B-B05D-BC49-8081-53356B529C14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FF30A4-4EE7-7048-82E4-EF799901FEA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plastics ingestion records fish" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8548" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8548" uniqueCount="1290">
   <si>
     <t>Species name</t>
   </si>
@@ -3848,9 +3848,6 @@
   </si>
   <si>
     <t>CARB</t>
-  </si>
-  <si>
-    <t>BRPL</t>
   </si>
   <si>
     <t>GUIA</t>
@@ -4825,8 +4822,8 @@
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A462" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A469" sqref="A469:A471"/>
+      <pane ySplit="1" topLeftCell="A452" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32156,7 +32153,7 @@
         <v>46</v>
       </c>
       <c r="AA349" s="10" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="AB349" t="s">
         <v>709</v>
@@ -32228,7 +32225,7 @@
         <v>21</v>
       </c>
       <c r="AA350" s="10" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="AB350" t="s">
         <v>709</v>
@@ -36082,7 +36079,7 @@
         <v>29</v>
       </c>
       <c r="AA396" s="10" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AB396" t="s">
         <v>779</v>
@@ -36168,7 +36165,7 @@
         <v>60</v>
       </c>
       <c r="AA397" s="10" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AB397" t="s">
         <v>1177</v>
@@ -36249,7 +36246,7 @@
         <v>38</v>
       </c>
       <c r="AA398" s="10" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AB398" t="s">
         <v>1177</v>
@@ -36321,7 +36318,7 @@
         <v>18</v>
       </c>
       <c r="AA399" s="10" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AB399" t="s">
         <v>1177</v>
@@ -36395,7 +36392,7 @@
         <v>26</v>
       </c>
       <c r="AA400" s="10" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AB400" t="s">
         <v>1177</v>
@@ -36464,7 +36461,7 @@
         <v>37</v>
       </c>
       <c r="AA401" s="10" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AB401" t="s">
         <v>1177</v>
@@ -36719,7 +36716,7 @@
         <v>17</v>
       </c>
       <c r="AA404" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB404" t="s">
         <v>418</v>
@@ -36897,7 +36894,7 @@
         <v>38</v>
       </c>
       <c r="AA406" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB406" t="s">
         <v>418</v>
@@ -36984,7 +36981,7 @@
         <v>35</v>
       </c>
       <c r="AA407" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB407" t="s">
         <v>418</v>
@@ -37331,7 +37328,7 @@
         <v>30</v>
       </c>
       <c r="AA411" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB411" t="s">
         <v>418</v>
@@ -37420,7 +37417,7 @@
         <v>21</v>
       </c>
       <c r="AA412" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB412" t="s">
         <v>418</v>
@@ -37954,7 +37951,7 @@
         <v>14</v>
       </c>
       <c r="AA418" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB418" t="s">
         <v>418</v>
@@ -38043,7 +38040,7 @@
         <v>22</v>
       </c>
       <c r="AA419" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB419" t="s">
         <v>418</v>
@@ -38132,7 +38129,7 @@
         <v>18</v>
       </c>
       <c r="AA420" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB420" t="s">
         <v>418</v>
@@ -38219,7 +38216,7 @@
         <v>21</v>
       </c>
       <c r="AA421" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB421" t="s">
         <v>418</v>
@@ -38308,7 +38305,7 @@
         <v>10</v>
       </c>
       <c r="AA422" s="10" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AB422" t="s">
         <v>418</v>
@@ -39193,7 +39190,7 @@
         <v>40</v>
       </c>
       <c r="AA433" s="10" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="AB433" t="s">
         <v>418</v>
@@ -40546,7 +40543,7 @@
         <v>17</v>
       </c>
       <c r="AA451" s="10" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="AB451" t="s">
         <v>1175</v>
@@ -40623,7 +40620,7 @@
         <v>14</v>
       </c>
       <c r="AA452" s="10" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="AB452" t="s">
         <v>1175</v>
@@ -41142,7 +41139,7 @@
         <v>22</v>
       </c>
       <c r="AA459" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB459" s="9" t="s">
         <v>1176</v>
@@ -41220,7 +41217,7 @@
         <v>26</v>
       </c>
       <c r="AA460" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB460" s="9" t="s">
         <v>1176</v>
@@ -41298,7 +41295,7 @@
         <v>34</v>
       </c>
       <c r="AA461" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB461" s="9" t="s">
         <v>1176</v>
@@ -41377,7 +41374,7 @@
         <v>25</v>
       </c>
       <c r="AA462" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB462" s="9" t="s">
         <v>1176</v>
@@ -41456,7 +41453,7 @@
         <v>12</v>
       </c>
       <c r="AA463" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB463" s="9" t="s">
         <v>1176</v>
@@ -41535,7 +41532,7 @@
         <v>17</v>
       </c>
       <c r="AA464" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB464" s="9" t="s">
         <v>1176</v>
@@ -41616,7 +41613,7 @@
         <v>34</v>
       </c>
       <c r="AA465" s="10" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AB465" s="9" t="s">
         <v>1176</v>
@@ -41871,7 +41868,7 @@
         <v>896</v>
       </c>
       <c r="B469" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C469" t="s">
         <v>159</v>
@@ -41933,16 +41930,16 @@
       </c>
       <c r="AC469" s="9"/>
       <c r="AD469" s="5" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AE469" s="9">
         <v>2018</v>
       </c>
       <c r="AF469" s="9" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AG469" s="9" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="470" spans="1:33" x14ac:dyDescent="0.2">
@@ -41950,7 +41947,7 @@
         <v>286</v>
       </c>
       <c r="B470" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C470" t="s">
         <v>159</v>
@@ -41972,10 +41969,10 @@
         <v>0.74242424242424243</v>
       </c>
       <c r="K470" t="s">
+        <v>1285</v>
+      </c>
+      <c r="L470" t="s">
         <v>1286</v>
-      </c>
-      <c r="L470" t="s">
-        <v>1287</v>
       </c>
       <c r="O470" t="s">
         <v>28</v>
@@ -42020,24 +42017,24 @@
         <v>2017</v>
       </c>
       <c r="AF470" s="9" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="AG470" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="471" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A471" s="18" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B471" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C471" s="17" t="s">
         <v>351</v>
       </c>
       <c r="D471" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="F471">
         <v>3.5</v>
@@ -42053,7 +42050,7 @@
         <v>0.2</v>
       </c>
       <c r="K471" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="L471" t="s">
         <v>810</v>
@@ -42102,10 +42099,10 @@
         <v>2017</v>
       </c>
       <c r="AF471" s="9" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="AG471" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="472" spans="1:33" x14ac:dyDescent="0.2">

</xml_diff>